<commit_message>
Implemented Add Resource Class and other helper functions
</commit_message>
<xml_diff>
--- a/API Doc.xlsx
+++ b/API Doc.xlsx
@@ -126,12 +126,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -161,13 +167,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -465,7 +472,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -493,7 +500,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="45">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -510,7 +517,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="60">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">

</xml_diff>

<commit_message>
Fixed some code issue
</commit_message>
<xml_diff>
--- a/API Doc.xlsx
+++ b/API Doc.xlsx
@@ -167,7 +167,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -175,6 +175,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -472,7 +473,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A3"/>
+      <selection activeCell="A3" sqref="A3:A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -517,7 +518,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="60">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -534,7 +535,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="75">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -551,7 +552,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="45">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -568,7 +569,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="60">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -585,7 +586,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="75">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">

</xml_diff>